<commit_message>
add rule builder, update Index Controller
</commit_message>
<xml_diff>
--- a/TestProject/TestProject/wwwroot/upload/Sheet1_1.xlsx
+++ b/TestProject/TestProject/wwwroot/upload/Sheet1_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\GraduationAssesment\TestProject\TestProject\wwwroot\upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/GraduationAssessment/GraduationAssesment/TestProject/TestProject/wwwroot/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905A581C-6117-4A12-8748-04F2B3D10151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A69E6C9-8C66-8348-ADED-5729E2E13E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" xr2:uid="{00E3A524-EC4E-456D-BA7B-A22EDF3283C9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22140" windowHeight="13320" xr2:uid="{00E3A524-EC4E-456D-BA7B-A22EDF3283C9}"/>
   </bookViews>
   <sheets>
     <sheet name="학생성적정보" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="239">
   <si>
     <t>순번</t>
   </si>
@@ -793,10 +793,6 @@
   </si>
   <si>
     <t>이강우</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>NEW재수강</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -807,7 +803,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1343,37 +1339,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB850E5-4B36-4BA0-B5F9-6B95E4DE2680}">
   <dimension ref="B1:W50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.600000000000001" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="2" max="2" width="4.640625" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="2" max="3" width="4.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
-    <col min="8" max="8" width="2.640625" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" customWidth="1"/>
+    <col min="9" max="9" width="25.83203125" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
     <col min="11" max="11" width="4.5" customWidth="1"/>
-    <col min="12" max="12" width="4.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.35546875" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" customWidth="1"/>
+    <col min="12" max="12" width="4.1640625" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" customWidth="1"/>
-    <col min="18" max="18" width="11.640625" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" customWidth="1"/>
+    <col min="17" max="17" width="7.83203125" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" customWidth="1"/>
+    <col min="19" max="19" width="9.83203125" customWidth="1"/>
     <col min="20" max="20" width="15.5" customWidth="1"/>
     <col min="21" max="21" width="22" customWidth="1"/>
-    <col min="22" max="22" width="25.85546875" customWidth="1"/>
-    <col min="23" max="23" width="8.640625" customWidth="1"/>
+    <col min="22" max="22" width="25.83203125" customWidth="1"/>
+    <col min="23" max="23" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:23" ht="28">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1441,7 +1436,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:23">
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -1501,7 +1496,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:23">
       <c r="B3" s="9">
         <v>2</v>
       </c>
@@ -1555,7 +1550,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:23" ht="28">
       <c r="B4" s="15">
         <v>3</v>
       </c>
@@ -1609,7 +1604,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:23" ht="28">
       <c r="B5" s="9">
         <v>4</v>
       </c>
@@ -1665,7 +1660,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:23">
       <c r="B6" s="15">
         <v>5</v>
       </c>
@@ -1721,7 +1716,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:23">
       <c r="B7" s="9">
         <v>6</v>
       </c>
@@ -1775,7 +1770,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:23" ht="28">
       <c r="B8" s="15">
         <v>7</v>
       </c>
@@ -1829,7 +1824,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:23">
       <c r="B9" s="9">
         <v>8</v>
       </c>
@@ -1889,7 +1884,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:23" ht="28">
       <c r="B10" s="15">
         <v>9</v>
       </c>
@@ -1943,7 +1938,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:23" ht="28">
       <c r="B11" s="9">
         <v>10</v>
       </c>
@@ -1997,7 +1992,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:23">
       <c r="B12" s="15">
         <v>11</v>
       </c>
@@ -2051,7 +2046,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:23" ht="28">
       <c r="B13" s="9">
         <v>12</v>
       </c>
@@ -2107,7 +2102,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:23" ht="28">
       <c r="B14" s="15">
         <v>13</v>
       </c>
@@ -2165,7 +2160,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:23">
       <c r="B15" s="9">
         <v>14</v>
       </c>
@@ -2219,7 +2214,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:23" ht="28">
       <c r="B16" s="15">
         <v>15</v>
       </c>
@@ -2273,7 +2268,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:23">
       <c r="B17" s="9">
         <v>16</v>
       </c>
@@ -2327,7 +2322,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:23">
       <c r="B18" s="15">
         <v>17</v>
       </c>
@@ -2381,7 +2376,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:23">
       <c r="B19" s="9">
         <v>18</v>
       </c>
@@ -2435,7 +2430,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:23">
       <c r="B20" s="15">
         <v>19</v>
       </c>
@@ -2491,7 +2486,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:23" ht="28">
       <c r="B21" s="9">
         <v>20</v>
       </c>
@@ -2545,7 +2540,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:23">
       <c r="B22" s="15">
         <v>21</v>
       </c>
@@ -2601,7 +2596,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:23">
       <c r="B23" s="15">
         <v>23</v>
       </c>
@@ -2655,7 +2650,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:23">
       <c r="B24" s="9">
         <v>24</v>
       </c>
@@ -2713,7 +2708,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:23" ht="28">
       <c r="B25" s="15">
         <v>25</v>
       </c>
@@ -2769,7 +2764,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:23">
       <c r="B26" s="9">
         <v>26</v>
       </c>
@@ -2823,7 +2818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:23" ht="28">
       <c r="B27" s="15">
         <v>27</v>
       </c>
@@ -2877,7 +2872,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:23">
       <c r="B28" s="9">
         <v>28</v>
       </c>
@@ -2931,7 +2926,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:23">
       <c r="B29" s="15">
         <v>29</v>
       </c>
@@ -2987,7 +2982,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:23" ht="28">
       <c r="B30" s="9">
         <v>30</v>
       </c>
@@ -3041,7 +3036,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:23">
       <c r="B31" s="15">
         <v>31</v>
       </c>
@@ -3095,7 +3090,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:23">
       <c r="B32" s="9">
         <v>32</v>
       </c>
@@ -3149,7 +3144,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:23">
       <c r="B33" s="15">
         <v>33</v>
       </c>
@@ -3203,7 +3198,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:23">
       <c r="B34" s="9">
         <v>34</v>
       </c>
@@ -3257,7 +3252,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:23" ht="28">
       <c r="B35" s="15">
         <v>35</v>
       </c>
@@ -3311,7 +3306,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="2:23" ht="23.15" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:23" ht="28">
       <c r="B36" s="9">
         <v>36</v>
       </c>
@@ -3367,7 +3362,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:23">
       <c r="C37">
         <v>2021</v>
       </c>
@@ -3405,7 +3400,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:23">
       <c r="E38" s="21" t="s">
         <v>197</v>
       </c>
@@ -3434,7 +3429,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="2:23">
       <c r="E39" s="22" t="s">
         <v>203</v>
       </c>
@@ -3457,7 +3452,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:23">
       <c r="E40" s="21" t="s">
         <v>203</v>
       </c>
@@ -3480,7 +3475,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:23">
       <c r="E41" s="22" t="s">
         <v>203</v>
       </c>
@@ -3503,7 +3498,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:23">
       <c r="E42" s="21" t="s">
         <v>203</v>
       </c>
@@ -3526,7 +3521,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="2:23">
       <c r="E43" s="22" t="s">
         <v>203</v>
       </c>
@@ -3552,7 +3547,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="2:23">
       <c r="E44" s="21" t="s">
         <v>203</v>
       </c>
@@ -3575,7 +3570,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="2:23">
       <c r="C45">
         <v>2022</v>
       </c>
@@ -3604,7 +3599,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="2:23">
       <c r="E46" s="21" t="s">
         <v>203</v>
       </c>
@@ -3627,7 +3622,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="2:23">
       <c r="E47" s="22" t="s">
         <v>203</v>
       </c>
@@ -3653,7 +3648,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="2:23">
       <c r="E48" s="21" t="s">
         <v>203</v>
       </c>
@@ -3676,7 +3671,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:23">
       <c r="E49" s="22" t="s">
         <v>203</v>
       </c>
@@ -3699,7 +3694,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:23">
       <c r="B50" s="9">
         <v>22</v>
       </c>
@@ -3728,9 +3723,7 @@
       </c>
       <c r="L50" s="11"/>
       <c r="M50" s="9"/>
-      <c r="N50" s="11" t="s">
-        <v>239</v>
-      </c>
+      <c r="N50" s="11"/>
       <c r="O50" s="11" t="s">
         <v>30</v>
       </c>

</xml_diff>